<commit_message>
update test data for sample ID change
</commit_message>
<xml_diff>
--- a/test/test_data/umi-T_N-PanCancer/test_manifest.xlsx
+++ b/test/test_data/umi-T_N-PanCancer/test_manifest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-9760" yWindow="-21140" windowWidth="38400" windowHeight="21040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SampleInfo" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
   <si>
     <t>CMO_SAMPLE_ID</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Test_Run</t>
   </si>
   <si>
-    <t>test_sample_1_N_IGO_TEST</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>test_patient_3</t>
   </si>
   <si>
-    <t>test_sample_6_T_sample_id_change_test</t>
-  </si>
-  <si>
     <t>bc409-bc409</t>
   </si>
   <si>
@@ -219,7 +213,43 @@
     <t>NewName</t>
   </si>
   <si>
-    <t>test_sample_2_T_new_name_test</t>
+    <t>test_investigator_sample_5_N</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_6_T</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_3_N</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_4_T</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_2_T</t>
+  </si>
+  <si>
+    <t>test_sample_4_T_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_1_N_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_2_T_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_3_N_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_6_T_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_5_N_IGO</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_1_N</t>
+  </si>
+  <si>
+    <t>test_sample_1_N</t>
   </si>
 </sst>
 </file>
@@ -569,7 +599,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,13 +688,13 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -735,13 +765,13 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -750,7 +780,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -768,13 +798,13 @@
         <v>33</v>
       </c>
       <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
-        <v>44</v>
-      </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O3">
         <v>7.6779999999999999</v>
@@ -812,13 +842,13 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -845,13 +875,13 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" t="s">
         <v>47</v>
       </c>
-      <c r="M4" t="s">
-        <v>48</v>
-      </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O4">
         <v>10</v>
@@ -889,13 +919,13 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -904,7 +934,7 @@
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -919,16 +949,16 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
         <v>50</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>51</v>
       </c>
-      <c r="M5" t="s">
-        <v>52</v>
-      </c>
       <c r="N5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O5">
         <v>10</v>
@@ -966,13 +996,13 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -999,13 +1029,13 @@
         <v>33</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -1043,13 +1073,13 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1058,7 +1088,7 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
         <v>30</v>
@@ -1073,16 +1103,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O7">
         <v>10</v>
@@ -1128,7 +1158,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,58 +1169,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>41</v>
+      <c r="A3" t="s">
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>45</v>
+      <c r="A4" t="s">
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>49</v>
+      <c r="A5" t="s">
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
+      <c r="A6" t="s">
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
+      <c r="A7" t="s">
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test data for one sample ID is substring of another sample ID
</commit_message>
<xml_diff>
--- a/test/test_data/umi-T_N-PanCancer/test_manifest.xlsx
+++ b/test/test_data/umi-T_N-PanCancer/test_manifest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="10580" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SampleInfo" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>LANE_NUMBER</t>
   </si>
   <si>
-    <t>test_sample_2_T</t>
-  </si>
-  <si>
     <t>test_patient_1</t>
   </si>
   <si>
@@ -225,18 +222,9 @@
     <t>test_investigator_sample_4_T</t>
   </si>
   <si>
-    <t>test_investigator_sample_2_T</t>
-  </si>
-  <si>
     <t>test_sample_4_T_IGO</t>
   </si>
   <si>
-    <t>test_sample_1_N_IGO</t>
-  </si>
-  <si>
-    <t>test_sample_2_T_IGO</t>
-  </si>
-  <si>
     <t>test_sample_3_N_IGO</t>
   </si>
   <si>
@@ -246,16 +234,28 @@
     <t>test_sample_5_N_IGO</t>
   </si>
   <si>
-    <t>test_investigator_sample_1_N</t>
-  </si>
-  <si>
-    <t>test_sample_1_N</t>
-  </si>
-  <si>
     <t>PROJECT_ID</t>
   </si>
   <si>
     <t>Test_Project</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_1a</t>
+  </si>
+  <si>
+    <t>test_investigator_sample_1</t>
+  </si>
+  <si>
+    <t>test_sample_1a_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_1_IGO</t>
+  </si>
+  <si>
+    <t>test_sample_1a</t>
+  </si>
+  <si>
+    <t>test_sample_1</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,51 +700,51 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
-        <v>35</v>
-      </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2">
         <v>7.9580000000000002</v>
@@ -756,75 +756,75 @@
         <v>500</v>
       </c>
       <c r="R2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S2">
         <v>7.6443000000000003</v>
       </c>
       <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
         <v>37</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>38</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="W2" t="s">
-        <v>40</v>
-      </c>
       <c r="X2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y2">
         <v>1</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O3">
         <v>7.6779999999999999</v>
@@ -836,75 +836,75 @@
         <v>500</v>
       </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S3">
         <v>7.6443000000000003</v>
       </c>
       <c r="T3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" t="s">
         <v>37</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>38</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>39</v>
       </c>
-      <c r="W3" t="s">
-        <v>40</v>
-      </c>
       <c r="X3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" t="s">
         <v>46</v>
       </c>
-      <c r="M4" t="s">
-        <v>47</v>
-      </c>
       <c r="N4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O4">
         <v>10</v>
@@ -916,75 +916,75 @@
         <v>500</v>
       </c>
       <c r="R4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S4">
         <v>7.6443000000000003</v>
       </c>
       <c r="T4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" t="s">
         <v>37</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>38</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>39</v>
       </c>
-      <c r="W4" t="s">
-        <v>40</v>
-      </c>
       <c r="X4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y4">
         <v>1</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" t="s">
         <v>49</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>50</v>
       </c>
-      <c r="M5" t="s">
-        <v>51</v>
-      </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O5">
         <v>10</v>
@@ -996,75 +996,75 @@
         <v>500</v>
       </c>
       <c r="R5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S5">
         <v>7.6443000000000003</v>
       </c>
       <c r="T5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" t="s">
         <v>37</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>38</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>39</v>
       </c>
-      <c r="W5" t="s">
-        <v>40</v>
-      </c>
       <c r="X5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y5">
         <v>1</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" t="s">
         <v>54</v>
       </c>
-      <c r="M6" t="s">
-        <v>55</v>
-      </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -1076,75 +1076,75 @@
         <v>500</v>
       </c>
       <c r="R6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S6">
         <v>7.6443000000000003</v>
       </c>
       <c r="T6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" t="s">
         <v>37</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>38</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>39</v>
       </c>
-      <c r="W6" t="s">
-        <v>40</v>
-      </c>
       <c r="X6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y6">
         <v>1</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>31</v>
-      </c>
-      <c r="I7" t="s">
-        <v>32</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" t="s">
         <v>57</v>
       </c>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O7">
         <v>10</v>
@@ -1156,31 +1156,31 @@
         <v>500</v>
       </c>
       <c r="R7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S7">
         <v>7.6443000000000003</v>
       </c>
       <c r="T7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" t="s">
         <v>37</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>38</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>39</v>
       </c>
-      <c r="W7" t="s">
-        <v>40</v>
-      </c>
       <c r="X7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y7">
         <v>1</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1204,58 +1204,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>